<commit_message>
Final version of MLP with PCA.
</commit_message>
<xml_diff>
--- a/benchmark.xlsx
+++ b/benchmark.xlsx
@@ -9855,7 +9855,7 @@
   <dimension ref="A1:L201"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9872,14 +9872,26 @@
         <v>0.05</v>
       </c>
       <c r="C1" s="2">
-        <v>0.05</v>
-      </c>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="D1" s="2">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="E1" s="2">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="F1" s="2">
+        <v>0.08</v>
+      </c>
+      <c r="G1" s="2">
+        <v>0.08</v>
+      </c>
+      <c r="H1" s="2">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="I1" s="2">
+        <v>7.0000000000000007E-2</v>
+      </c>
       <c r="J1" s="2"/>
       <c r="K1" s="2"/>
       <c r="L1" s="2"/>
@@ -9894,12 +9906,24 @@
       <c r="C2" s="3">
         <v>0.01</v>
       </c>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
+      <c r="D2" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="E2" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="F2" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="G2" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="H2" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="I2" s="3">
+        <v>0.01</v>
+      </c>
       <c r="J2" s="3"/>
       <c r="K2" s="3"/>
       <c r="L2" s="3"/>
@@ -9911,13 +9935,27 @@
       <c r="B3" s="3">
         <v>10</v>
       </c>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
+      <c r="C3" s="3">
+        <v>10</v>
+      </c>
+      <c r="D3" s="3">
+        <v>10</v>
+      </c>
+      <c r="E3" s="3">
+        <v>10</v>
+      </c>
+      <c r="F3" s="3">
+        <v>10</v>
+      </c>
+      <c r="G3" s="3">
+        <v>10</v>
+      </c>
+      <c r="H3" s="3">
+        <v>10</v>
+      </c>
+      <c r="I3" s="3">
+        <v>10</v>
+      </c>
       <c r="J3" s="3"/>
       <c r="K3" s="3"/>
       <c r="L3" s="3"/>
@@ -9929,13 +9967,27 @@
       <c r="B4" s="3">
         <v>1000</v>
       </c>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
+      <c r="C4" s="3">
+        <v>2000</v>
+      </c>
+      <c r="D4" s="3">
+        <v>2000</v>
+      </c>
+      <c r="E4" s="3">
+        <v>3000</v>
+      </c>
+      <c r="F4" s="3">
+        <v>5000</v>
+      </c>
+      <c r="G4" s="3">
+        <v>10000</v>
+      </c>
+      <c r="H4" s="3">
+        <v>10000</v>
+      </c>
+      <c r="I4" s="3">
+        <v>42000</v>
+      </c>
       <c r="J4" s="3"/>
       <c r="K4" s="3"/>
       <c r="L4" s="3"/>
@@ -9947,13 +9999,27 @@
       <c r="B5" s="3">
         <v>0.85329999999999995</v>
       </c>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
+      <c r="C5" s="3">
+        <v>0.86</v>
+      </c>
+      <c r="D5" s="3">
+        <v>0.84833000000000003</v>
+      </c>
+      <c r="E5" s="3">
+        <v>0.85109999999999997</v>
+      </c>
+      <c r="F5" s="3">
+        <v>0.86799999999999999</v>
+      </c>
+      <c r="G5" s="3">
+        <v>0.85260000000000002</v>
+      </c>
+      <c r="H5" s="3">
+        <v>0.85329999999999995</v>
+      </c>
+      <c r="I5" s="3">
+        <v>0.87909999999999999</v>
+      </c>
       <c r="J5" s="3"/>
       <c r="K5" s="3"/>
       <c r="L5" s="3"/>
@@ -9965,13 +10031,27 @@
       <c r="B6" s="3">
         <v>40.6113</v>
       </c>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
+      <c r="C6" s="3">
+        <v>27</v>
+      </c>
+      <c r="D6" s="3">
+        <v>26.7</v>
+      </c>
+      <c r="E6" s="3">
+        <v>26.9</v>
+      </c>
+      <c r="F6" s="3">
+        <v>26.87</v>
+      </c>
+      <c r="G6" s="3">
+        <v>19.86</v>
+      </c>
+      <c r="H6" s="3">
+        <v>24.41</v>
+      </c>
+      <c r="I6" s="3">
+        <v>39</v>
+      </c>
       <c r="J6" s="3"/>
       <c r="K6" s="3"/>
       <c r="L6" s="3"/>
@@ -9980,575 +10060,1244 @@
       <c r="B7" s="4">
         <v>5.0110826470600003</v>
       </c>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
+      <c r="C7" s="4">
+        <v>3.2058508468600002</v>
+      </c>
+      <c r="D7" s="4">
+        <v>3.2571381102000001</v>
+      </c>
+      <c r="E7">
+        <v>2.2363594841599999</v>
+      </c>
+      <c r="F7">
+        <v>1.5027562243599999</v>
+      </c>
+      <c r="G7">
+        <v>0.88107676167899995</v>
+      </c>
+      <c r="H7">
+        <v>0.86808912533799998</v>
+      </c>
+      <c r="I7">
+        <v>0.31509557605499999</v>
+      </c>
       <c r="L7" s="3"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B8" s="4">
         <v>0.95572665643200005</v>
       </c>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
+      <c r="C8" s="4">
+        <v>0.33080989937999999</v>
+      </c>
+      <c r="D8" s="4">
+        <v>0.30302129236800002</v>
+      </c>
+      <c r="E8">
+        <v>0.16047655929900001</v>
+      </c>
+      <c r="F8">
+        <v>0.112489707792</v>
+      </c>
+      <c r="G8">
+        <v>9.0734239627999994E-2</v>
+      </c>
+      <c r="H8">
+        <v>0.106572899382</v>
+      </c>
+      <c r="I8">
+        <v>0.15276374786399999</v>
+      </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B9" s="4">
         <v>0.38878243435499998</v>
       </c>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
+      <c r="C9" s="4">
+        <v>0.152027023535</v>
+      </c>
+      <c r="D9" s="4">
+        <v>0.129558553765</v>
+      </c>
+      <c r="E9">
+        <v>8.5910829802900004E-2</v>
+      </c>
+      <c r="F9">
+        <v>0.10338944322599999</v>
+      </c>
+      <c r="G9">
+        <v>0.13047879565000001</v>
+      </c>
+      <c r="H9">
+        <v>0.15333198891700001</v>
+      </c>
+      <c r="I9">
+        <v>9.6804142683600006E-2</v>
+      </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B10" s="4">
         <v>0.215718651772</v>
       </c>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
+      <c r="C10" s="4">
+        <v>0.10980120598900001</v>
+      </c>
+      <c r="D10" s="4">
+        <v>9.1218730521599997E-2</v>
+      </c>
+      <c r="E10">
+        <v>7.53179548556E-2</v>
+      </c>
+      <c r="F10">
+        <v>0.12623111460399999</v>
+      </c>
+      <c r="G10">
+        <v>0.159918873027</v>
+      </c>
+      <c r="H10">
+        <v>0.16499102045399999</v>
+      </c>
+      <c r="I10">
+        <v>7.0518594195800005E-2</v>
+      </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B11" s="4">
         <v>0.14454833476199999</v>
       </c>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
+      <c r="C11" s="4">
+        <v>9.7650839174699994E-2</v>
+      </c>
+      <c r="D11" s="4">
+        <v>8.2331194712399997E-2</v>
+      </c>
+      <c r="E11">
+        <v>7.9385791099799999E-2</v>
+      </c>
+      <c r="F11">
+        <v>0.14877356834800001</v>
+      </c>
+      <c r="G11">
+        <v>0.164501570864</v>
+      </c>
+      <c r="H11">
+        <v>0.15870573411399999</v>
+      </c>
+      <c r="I11">
+        <v>5.6831463220600002E-2</v>
+      </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B12" s="4">
         <v>0.11051228219000001</v>
       </c>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
+      <c r="C12" s="4">
+        <v>9.7092953741300003E-2</v>
+      </c>
+      <c r="D12" s="4">
+        <v>8.4846984202699996E-2</v>
+      </c>
+      <c r="E12">
+        <v>8.9372209983300005E-2</v>
+      </c>
+      <c r="F12">
+        <v>0.16217199886</v>
+      </c>
+      <c r="G12">
+        <v>0.15065152927</v>
+      </c>
+      <c r="H12">
+        <v>0.14656990323800001</v>
+      </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B13" s="4">
         <v>9.2870874827400002E-2</v>
       </c>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
+      <c r="C13" s="4">
+        <v>0.10290052747</v>
+      </c>
+      <c r="D13" s="4">
+        <v>9.3455766077500002E-2</v>
+      </c>
+      <c r="E13">
+        <v>0.101515681835</v>
+      </c>
+      <c r="F13">
+        <v>0.16879903601400001</v>
+      </c>
+      <c r="G13">
+        <v>0.13283966648199999</v>
+      </c>
+      <c r="H13">
+        <v>0.13359360717999999</v>
+      </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B14" s="4">
         <v>8.3516846291499997E-2</v>
       </c>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
+      <c r="C14" s="4">
+        <v>0.11256482681799999</v>
+      </c>
+      <c r="D14" s="4">
+        <v>0.105423189672</v>
+      </c>
+      <c r="E14">
+        <v>0.114160237483</v>
+      </c>
+      <c r="F14">
+        <v>0.170897954139</v>
+      </c>
+      <c r="G14">
+        <v>0.11722303414099999</v>
+      </c>
+      <c r="H14">
+        <v>0.12081348240299999</v>
+      </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B15" s="4">
         <v>7.8861554669799994E-2</v>
       </c>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
+      <c r="C15" s="4">
+        <v>0.124259840042</v>
+      </c>
+      <c r="D15" s="4">
+        <v>0.118791308883</v>
+      </c>
+      <c r="E15">
+        <v>0.12648435642899999</v>
+      </c>
+      <c r="F15">
+        <v>0.169682495952</v>
+      </c>
+      <c r="G15">
+        <v>0.104556980322</v>
+      </c>
+      <c r="H15">
+        <v>0.108598984715</v>
+      </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B16" s="4">
         <v>7.7174695588200004E-2</v>
       </c>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
-    </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C16" s="4">
+        <v>0.13653745428799999</v>
+      </c>
+      <c r="D16" s="4">
+        <v>0.132122916768</v>
+      </c>
+      <c r="E16">
+        <v>0.13787159697699999</v>
+      </c>
+      <c r="F16">
+        <v>0.16610567515499999</v>
+      </c>
+      <c r="G16">
+        <v>9.4274706621299997E-2</v>
+      </c>
+      <c r="H16">
+        <v>9.7702582555199993E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B17" s="4">
         <v>7.7563015670299995E-2</v>
       </c>
-      <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
-    </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C17" s="4">
+        <v>0.148331428185</v>
+      </c>
+      <c r="D17" s="4">
+        <v>0.14442689123899999</v>
+      </c>
+      <c r="E17">
+        <v>0.147848352973</v>
+      </c>
+      <c r="F17">
+        <v>0.16099222474399999</v>
+      </c>
+      <c r="G17">
+        <v>8.57688342996E-2</v>
+      </c>
+      <c r="H17">
+        <v>8.85156274805E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B18" s="4">
         <v>7.9531818504500001E-2</v>
       </c>
-      <c r="C18" s="4"/>
-      <c r="D18" s="4"/>
-    </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C18" s="4">
+        <v>0.158945204989</v>
+      </c>
+      <c r="D18" s="4">
+        <v>0.155071812245</v>
+      </c>
+      <c r="E18">
+        <v>0.15604990488500001</v>
+      </c>
+      <c r="F18">
+        <v>0.155043222003</v>
+      </c>
+      <c r="G18">
+        <v>7.8612558554100001E-2</v>
+      </c>
+      <c r="H18">
+        <v>8.0933016160700005E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B19" s="4">
         <v>8.2780741813800005E-2</v>
       </c>
-      <c r="C19" s="4"/>
-      <c r="D19" s="4"/>
-    </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C19" s="4">
+        <v>0.16799037221300001</v>
+      </c>
+      <c r="D19" s="4">
+        <v>0.1637223951</v>
+      </c>
+      <c r="E19">
+        <v>0.162162751163</v>
+      </c>
+      <c r="F19">
+        <v>0.14880169269599999</v>
+      </c>
+      <c r="H19">
+        <v>7.4671177541699996E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B20" s="4">
         <v>8.7102803351799998E-2</v>
       </c>
-      <c r="C20" s="4"/>
-      <c r="D20" s="4"/>
-    </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C20" s="4">
+        <v>0.17530553551299999</v>
+      </c>
+      <c r="D20" s="4">
+        <v>0.17028516200999999</v>
+      </c>
+      <c r="E20">
+        <v>0.16597675003599999</v>
+      </c>
+      <c r="F20">
+        <v>0.14260812670799999</v>
+      </c>
+      <c r="H20">
+        <v>6.9454001350699998E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B21" s="4">
         <v>9.2332240200900001E-2</v>
       </c>
-      <c r="C21" s="4"/>
-      <c r="D21" s="4"/>
-    </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C21" s="4">
+        <v>0.18088313968700001</v>
+      </c>
+      <c r="D21" s="4">
+        <v>0.17483323429600001</v>
+      </c>
+      <c r="E21">
+        <v>0.16751687636199999</v>
+      </c>
+      <c r="F21">
+        <v>0.136614344937</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B22" s="4">
         <v>9.8316792915400006E-2</v>
       </c>
-      <c r="C22" s="4"/>
-      <c r="D22" s="4"/>
-    </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C22" s="4">
+        <v>0.184812095776</v>
+      </c>
+      <c r="D22" s="4">
+        <v>0.177526053628</v>
+      </c>
+      <c r="E22">
+        <v>0.16706362126499999</v>
+      </c>
+      <c r="F22">
+        <v>0.13086709186100001</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B23" s="4">
         <v>0.10490318517199999</v>
       </c>
-      <c r="C23" s="4"/>
-      <c r="D23" s="4"/>
-    </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C23" s="4">
+        <v>0.187235459745</v>
+      </c>
+      <c r="D23" s="4">
+        <v>0.17855804483099999</v>
+      </c>
+      <c r="E23">
+        <v>0.16504065494299999</v>
+      </c>
+      <c r="F23">
+        <v>0.12540030561000001</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B24" s="4">
         <v>0.111930609174</v>
       </c>
-      <c r="C24" s="4"/>
-      <c r="D24" s="4"/>
-    </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C24" s="4">
+        <v>0.18832271188399999</v>
+      </c>
+      <c r="D24" s="4">
+        <v>0.17814261255399999</v>
+      </c>
+      <c r="E24">
+        <v>0.16189051066900001</v>
+      </c>
+      <c r="F24">
+        <v>0.12026345308600001</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B25" s="4">
         <v>0.119229716395</v>
       </c>
-      <c r="C25" s="4"/>
-      <c r="D25" s="4"/>
-    </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C25" s="4">
+        <v>0.188254009592</v>
+      </c>
+      <c r="D25" s="4">
+        <v>0.17651124044899999</v>
+      </c>
+      <c r="E25">
+        <v>0.15799564604999999</v>
+      </c>
+      <c r="F25">
+        <v>0.11549277689699999</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B26" s="4">
         <v>0.126625580046</v>
       </c>
-      <c r="C26" s="4"/>
-      <c r="D26" s="4"/>
-    </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C26" s="4">
+        <v>0.187211054933</v>
+      </c>
+      <c r="D26" s="4">
+        <v>0.173908051344</v>
+      </c>
+      <c r="E26">
+        <v>0.153648802542</v>
+      </c>
+      <c r="F26">
+        <v>0.111083590128</v>
+      </c>
+    </row>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B27" s="4">
         <v>0.13394338392399999</v>
       </c>
-      <c r="C27" s="4"/>
-      <c r="D27" s="4"/>
-    </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C27" s="4">
+        <v>0.185370204925</v>
+      </c>
+      <c r="D27" s="4">
+        <v>0.17057540362699999</v>
+      </c>
+      <c r="E27">
+        <v>0.149062277055</v>
+      </c>
+      <c r="F27">
+        <v>0.10699164143500001</v>
+      </c>
+    </row>
+    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B28" s="4">
         <v>0.14101583959700001</v>
       </c>
-      <c r="C28" s="4"/>
-      <c r="D28" s="4"/>
-    </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C28" s="4">
+        <v>0.18289637725399999</v>
+      </c>
+      <c r="D28" s="4">
+        <v>0.16673654284299999</v>
+      </c>
+      <c r="E28">
+        <v>0.144390840908</v>
+      </c>
+      <c r="F28">
+        <v>0.10315223069600001</v>
+      </c>
+    </row>
+    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B29" s="4">
         <v>0.14769159966299999</v>
       </c>
-      <c r="C29" s="4"/>
-      <c r="D29" s="4"/>
-    </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C29" s="4">
+        <v>0.179938227506</v>
+      </c>
+      <c r="D29" s="4">
+        <v>0.16258245351699999</v>
+      </c>
+      <c r="E29">
+        <v>0.139748632101</v>
+      </c>
+      <c r="F29">
+        <v>9.9501143073099999E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B30" s="4">
         <v>0.153843866169</v>
       </c>
-      <c r="C30" s="4"/>
-      <c r="D30" s="4"/>
-    </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C30" s="4">
+        <v>0.17662538688400001</v>
+      </c>
+      <c r="D30" s="4">
+        <v>0.15826624358399999</v>
+      </c>
+      <c r="E30">
+        <v>0.13521804900100001</v>
+      </c>
+      <c r="F30">
+        <v>9.5990429790399998E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B31" s="4">
         <v>0.159377863856</v>
       </c>
-      <c r="C31" s="4"/>
-      <c r="D31" s="4"/>
-    </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C31" s="4">
+        <v>0.17306785887500001</v>
+      </c>
+      <c r="D31" s="4">
+        <v>0.15390419122599999</v>
+      </c>
+      <c r="E31">
+        <v>0.130855484405</v>
+      </c>
+      <c r="F31">
+        <v>9.2595515224100006E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B32" s="4">
         <v>0.164235386461</v>
       </c>
-      <c r="C32" s="4"/>
-      <c r="D32" s="4"/>
-    </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C32" s="4">
+        <v>0.16935686523599999</v>
+      </c>
+      <c r="D32" s="4">
+        <v>0.14958057216500001</v>
+      </c>
+      <c r="E32">
+        <v>0.12669651616899999</v>
+      </c>
+      <c r="F32">
+        <v>8.9312764591100005E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B33" s="4">
         <v>0.16839498031</v>
       </c>
-      <c r="C33" s="4"/>
-      <c r="D33" s="4"/>
-    </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C33" s="4">
+        <v>0.16556621828199999</v>
+      </c>
+      <c r="D33" s="4">
+        <v>0.145353693885</v>
+      </c>
+      <c r="E33">
+        <v>0.122760636053</v>
+      </c>
+      <c r="F33">
+        <v>8.6151459051099999E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B34" s="4">
         <v>0.17186760637000001</v>
       </c>
-      <c r="C34" s="4"/>
-      <c r="D34" s="4"/>
-    </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C34" s="4">
+        <v>0.161753730101</v>
+      </c>
+      <c r="D34" s="4">
+        <v>0.141261728886</v>
+      </c>
+      <c r="E34">
+        <v>0.11905512576299999</v>
+      </c>
+      <c r="F34">
+        <v>8.3125524999100003E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B35" s="4">
         <v>0.17468907394399999</v>
       </c>
-      <c r="C35" s="4"/>
-      <c r="D35" s="4"/>
-    </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C35" s="4">
+        <v>0.15796272749000001</v>
+      </c>
+      <c r="D35" s="4">
+        <v>0.13732780066399999</v>
+      </c>
+      <c r="E35">
+        <v>0.115578090903</v>
+      </c>
+      <c r="F35">
+        <v>8.0247869784800002E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B36" s="4">
         <v>0.17691129045500001</v>
       </c>
-      <c r="C36" s="4"/>
-      <c r="D36" s="4"/>
-    </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C36" s="4">
+        <v>0.15422393054799999</v>
+      </c>
+      <c r="D36" s="4">
+        <v>0.13356416427500001</v>
+      </c>
+      <c r="E36">
+        <v>0.11232095533399999</v>
+      </c>
+      <c r="F36">
+        <v>7.7527543293100007E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B37" s="4">
         <v>0.17859416694300001</v>
       </c>
-      <c r="C37" s="4"/>
-      <c r="D37" s="4"/>
-    </row>
-    <row r="38" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C37" s="4">
+        <v>0.15055774105200001</v>
+      </c>
+      <c r="D37" s="4">
+        <v>0.12997547894</v>
+      </c>
+      <c r="E37">
+        <v>0.109270675538</v>
+      </c>
+    </row>
+    <row r="38" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B38" s="4">
         <v>0.17979924862800001</v>
       </c>
-      <c r="C38" s="4"/>
-      <c r="D38" s="4"/>
-    </row>
-    <row r="39" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C38" s="4">
+        <v>0.14697669300800001</v>
+      </c>
+      <c r="D38" s="4">
+        <v>0.126561255165</v>
+      </c>
+      <c r="E38">
+        <v>0.106411713262</v>
+      </c>
+    </row>
+    <row r="39" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B39" s="4">
         <v>0.180585349496</v>
       </c>
-      <c r="C39" s="4"/>
-      <c r="D39" s="4"/>
-    </row>
-    <row r="40" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C39" s="4">
+        <v>0.14348771949200001</v>
+      </c>
+      <c r="D39" s="4">
+        <v>0.123317611892</v>
+      </c>
+      <c r="E39">
+        <v>0.103727655689</v>
+      </c>
+    </row>
+    <row r="40" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B40" s="4">
         <v>0.18100596715200001</v>
       </c>
-      <c r="C40" s="4"/>
-      <c r="D40" s="4"/>
-    </row>
-    <row r="41" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C40" s="4">
+        <v>0.14009400593400001</v>
+      </c>
+      <c r="D40" s="4">
+        <v>0.120238499634</v>
+      </c>
+      <c r="E40">
+        <v>0.10120240111000001</v>
+      </c>
+    </row>
+    <row r="41" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B41" s="4">
         <v>0.18110806243800001</v>
       </c>
-      <c r="C41" s="4"/>
-      <c r="D41" s="4"/>
-    </row>
-    <row r="42" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C41" s="4">
+        <v>0.136796379223</v>
+      </c>
+      <c r="D41" s="4">
+        <v>0.117316537163</v>
+      </c>
+      <c r="E41">
+        <v>9.8820932875800002E-2</v>
+      </c>
+    </row>
+    <row r="42" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B42" s="4">
         <v>0.18093179268500001</v>
       </c>
-      <c r="C42" s="4"/>
-      <c r="D42" s="4"/>
-    </row>
-    <row r="43" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C42" s="4">
+        <v>0.13359429532</v>
+      </c>
+      <c r="D42" s="4">
+        <v>0.114543583785</v>
+      </c>
+      <c r="E42">
+        <v>9.6569759268900005E-2</v>
+      </c>
+    </row>
+    <row r="43" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B43" s="4">
         <v>0.180510869101</v>
       </c>
-      <c r="C43" s="4"/>
-      <c r="D43" s="4"/>
-    </row>
-    <row r="44" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C43" s="4">
+        <v>0.13048651362300001</v>
+      </c>
+      <c r="D43" s="4">
+        <v>0.11191113817999999</v>
+      </c>
+      <c r="E43">
+        <v>9.4437090103900001E-2</v>
+      </c>
+    </row>
+    <row r="44" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B44" s="4">
         <v>0.17987329698499999</v>
       </c>
-      <c r="C44" s="4"/>
-      <c r="D44" s="4"/>
-    </row>
-    <row r="45" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C44" s="4">
+        <v>0.127471528542</v>
+      </c>
+      <c r="D44" s="4">
+        <v>0.109410625447</v>
+      </c>
+      <c r="E44">
+        <v>9.2412804215800004E-2</v>
+      </c>
+    </row>
+    <row r="45" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B45" s="4">
         <v>0.179042325162</v>
       </c>
-      <c r="C45" s="4"/>
-      <c r="D45" s="4"/>
-    </row>
-    <row r="46" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C45" s="4">
+        <v>0.124547810725</v>
+      </c>
+      <c r="D45" s="4">
+        <v>0.107033609861</v>
+      </c>
+      <c r="E45">
+        <v>9.0488263311500006E-2</v>
+      </c>
+    </row>
+    <row r="46" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B46" s="4">
         <v>0.17803747592399999</v>
       </c>
-      <c r="C46" s="4"/>
-      <c r="D46" s="4"/>
-    </row>
-    <row r="47" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C46" s="4">
+        <v>0.12171390535899999</v>
+      </c>
+      <c r="D46" s="4">
+        <v>0.104771953037</v>
+      </c>
+      <c r="E46">
+        <v>8.8656037360899997E-2</v>
+      </c>
+    </row>
+    <row r="47" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B47" s="4">
         <v>0.176875555377</v>
       </c>
-      <c r="C47" s="4"/>
-      <c r="D47" s="4"/>
-    </row>
-    <row r="48" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C47" s="4">
+        <v>0.118968435602</v>
+      </c>
+      <c r="D47" s="4">
+        <v>0.10261792626000001</v>
+      </c>
+      <c r="E47">
+        <v>8.6909608622199999E-2</v>
+      </c>
+    </row>
+    <row r="48" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B48" s="4">
         <v>0.17557156494500001</v>
       </c>
-      <c r="C48" s="4"/>
-      <c r="D48" s="4"/>
-    </row>
-    <row r="49" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C48" s="4">
+        <v>0.11631005625</v>
+      </c>
+      <c r="D48" s="4">
+        <v>0.100564280837</v>
+      </c>
+      <c r="E48">
+        <v>8.5243109932299999E-2</v>
+      </c>
+    </row>
+    <row r="49" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B49" s="4">
         <v>0.17413945474699999</v>
       </c>
-      <c r="C49" s="4"/>
-      <c r="D49" s="4"/>
-    </row>
-    <row r="50" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C49" s="4">
+        <v>0.113737393353</v>
+      </c>
+      <c r="D49" s="4">
+        <v>9.8604279961099994E-2</v>
+      </c>
+      <c r="E49">
+        <v>8.3651131000900006E-2</v>
+      </c>
+    </row>
+    <row r="50" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B50" s="4">
         <v>0.17259268220900001</v>
       </c>
-      <c r="C50" s="4"/>
-      <c r="D50" s="4"/>
-    </row>
-    <row r="51" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C50" s="4">
+        <v>0.11124899260399999</v>
+      </c>
+      <c r="D50" s="4">
+        <v>9.6731697521500001E-2</v>
+      </c>
+      <c r="E50">
+        <v>8.2128600995700005E-2</v>
+      </c>
+    </row>
+    <row r="51" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B51" s="4">
         <v>0.170944564567</v>
       </c>
-      <c r="C51" s="4"/>
-      <c r="D51" s="4"/>
-    </row>
-    <row r="52" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C51" s="4">
+        <v>0.108843286671</v>
+      </c>
+      <c r="D51" s="4">
+        <v>9.4940791485300005E-2</v>
+      </c>
+      <c r="E51">
+        <v>8.0670734943199998E-2</v>
+      </c>
+    </row>
+    <row r="52" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B52" s="4">
         <v>0.16920843857000001</v>
       </c>
-      <c r="C52" s="4"/>
-      <c r="D52" s="4"/>
-    </row>
-    <row r="53" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C52" s="4">
+        <v>0.10651858204</v>
+      </c>
+      <c r="D52" s="4">
+        <v>9.3226260833899996E-2</v>
+      </c>
+      <c r="E52">
+        <v>7.9273021196700003E-2</v>
+      </c>
+    </row>
+    <row r="53" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B53" s="4">
         <v>0.16739766040599999</v>
       </c>
-      <c r="C53" s="4"/>
-      <c r="D53" s="4"/>
-    </row>
-    <row r="54" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C53" s="4">
+        <v>0.104273060241</v>
+      </c>
+      <c r="D53" s="4">
+        <v>9.1583195021399999E-2</v>
+      </c>
+      <c r="E53">
+        <v>7.7931227568500003E-2</v>
+      </c>
+    </row>
+    <row r="54" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B54" s="4">
         <v>0.165525490464</v>
       </c>
-      <c r="C54" s="4"/>
-      <c r="D54" s="4"/>
-    </row>
-    <row r="55" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C54" s="4">
+        <v>0.10210478666099999</v>
+      </c>
+      <c r="D54" s="4">
+        <v>9.0007023831499999E-2</v>
+      </c>
+      <c r="E54">
+        <v>7.6641410300099994E-2</v>
+      </c>
+    </row>
+    <row r="55" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B55" s="4">
         <v>0.163604910184</v>
       </c>
-      <c r="C55" s="4"/>
-      <c r="D55" s="4"/>
-    </row>
-    <row r="56" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C55" s="4">
+        <v>0.10001172139599999</v>
+      </c>
+      <c r="D55" s="4">
+        <v>8.8493473644700005E-2</v>
+      </c>
+      <c r="E55">
+        <v>7.5399917803200003E-2</v>
+      </c>
+    </row>
+    <row r="56" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B56" s="4">
         <v>0.16164841352100001</v>
       </c>
-      <c r="C56" s="4"/>
-      <c r="D56" s="4"/>
-    </row>
-    <row r="57" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C56" s="4">
+        <v>9.7991729490500001E-2</v>
+      </c>
+      <c r="D56" s="4">
+        <v>8.7038533928200004E-2</v>
+      </c>
+      <c r="E56">
+        <v>7.4203386979299998E-2</v>
+      </c>
+    </row>
+    <row r="57" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B57" s="4">
         <v>0.15966780644699999</v>
       </c>
-      <c r="C57" s="4"/>
-      <c r="D57" s="4"/>
-    </row>
-    <row r="58" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C57" s="4">
+        <v>9.6042590826800001E-2</v>
+      </c>
+      <c r="D57" s="4">
+        <v>8.56384355204E-2</v>
+      </c>
+      <c r="E57">
+        <v>7.3048733145100006E-2</v>
+      </c>
+    </row>
+    <row r="58" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B58" s="4">
         <v>0.15767403717699999</v>
       </c>
-      <c r="C58" s="4"/>
-      <c r="D58" s="4"/>
-    </row>
-    <row r="59" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C58" s="4">
+        <v>9.4162011700899995E-2</v>
+      </c>
+      <c r="D58" s="4">
+        <v>8.4289640329800006E-2</v>
+      </c>
+      <c r="E58">
+        <v>7.1933135704199999E-2</v>
+      </c>
+    </row>
+    <row r="59" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B59" s="4">
         <v>0.155677069822</v>
       </c>
-      <c r="C59" s="4"/>
-      <c r="D59" s="4"/>
-    </row>
-    <row r="60" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C59" s="4">
+        <v>9.2347640340899997E-2</v>
+      </c>
+      <c r="D59" s="4">
+        <v>8.2988840625999996E-2</v>
+      </c>
+      <c r="E59">
+        <v>7.0854021620600005E-2</v>
+      </c>
+    </row>
+    <row r="60" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B60" s="4">
         <v>0.15368580589299999</v>
       </c>
-      <c r="C60" s="4"/>
-      <c r="D60" s="4"/>
-    </row>
-    <row r="61" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C60" s="4">
+        <v>9.0597087568900003E-2</v>
+      </c>
+      <c r="D60" s="4">
+        <v>8.1732965282299994E-2</v>
+      </c>
+      <c r="E60">
+        <v>6.9809048206999999E-2</v>
+      </c>
+    </row>
+    <row r="61" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B61" s="4">
         <v>0.15170805207099999</v>
       </c>
-      <c r="C61" s="4"/>
-      <c r="D61" s="4"/>
-    </row>
-    <row r="62" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C61" s="4">
+        <v>8.89079521821E-2</v>
+      </c>
+      <c r="D61" s="4">
+        <v>8.0519190038200003E-2</v>
+      </c>
+    </row>
+    <row r="62" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B62" s="4">
         <v>0.14975052864800001</v>
       </c>
-      <c r="C62" s="4"/>
-      <c r="D62" s="4"/>
-    </row>
-    <row r="63" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C62" s="4">
+        <v>8.7277849156799994E-2</v>
+      </c>
+      <c r="D62" s="4">
+        <v>7.9344948836699999E-2</v>
+      </c>
+    </row>
+    <row r="63" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B63" s="4">
         <v>0.147818910867</v>
       </c>
-      <c r="C63" s="4"/>
-      <c r="D63" s="4"/>
-    </row>
-    <row r="64" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C63" s="4">
+        <v>8.57044379341E-2</v>
+      </c>
+      <c r="D63" s="4">
+        <v>7.8207943342600006E-2</v>
+      </c>
+    </row>
+    <row r="64" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B64" s="4">
         <v>0.14591789451699999</v>
       </c>
-      <c r="C64" s="4"/>
-      <c r="D64" s="4"/>
+      <c r="C64" s="4">
+        <v>8.4185447979000003E-2</v>
+      </c>
+      <c r="D64" s="4">
+        <v>7.7106147840600006E-2</v>
+      </c>
     </row>
     <row r="65" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B65" s="4">
         <v>0.14405127738000001</v>
       </c>
-      <c r="C65" s="4"/>
-      <c r="D65" s="4"/>
+      <c r="C65" s="4">
+        <v>8.2718699395500001E-2</v>
+      </c>
+      <c r="D65" s="4">
+        <v>7.6037807032699994E-2</v>
+      </c>
     </row>
     <row r="66" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B66" s="4">
         <v>0.14222204898499999</v>
       </c>
-      <c r="C66" s="4"/>
-      <c r="D66" s="4"/>
+      <c r="C66" s="4">
+        <v>8.1302117338300006E-2</v>
+      </c>
+      <c r="D66" s="4">
+        <v>7.5001425007700004E-2</v>
+      </c>
     </row>
     <row r="67" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B67" s="4">
         <v>0.14043248250599999</v>
       </c>
-      <c r="C67" s="4"/>
-      <c r="D67" s="4"/>
+      <c r="C67" s="4">
+        <v>7.9933739960799999E-2</v>
+      </c>
+      <c r="D67" s="4">
+        <v>7.3995744892900006E-2</v>
+      </c>
     </row>
     <row r="68" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B68" s="4">
         <v>0.138684224168</v>
       </c>
-      <c r="C68" s="4"/>
-      <c r="D68" s="4"/>
+      <c r="C68" s="4">
+        <v>7.8611720433499996E-2</v>
+      </c>
+      <c r="D68" s="4">
+        <v>7.3019720183299996E-2</v>
+      </c>
     </row>
     <row r="69" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B69" s="4">
         <v>0.13697837712899999</v>
       </c>
-      <c r="C69" s="4"/>
-      <c r="D69" s="4"/>
+      <c r="C69" s="4">
+        <v>7.7334324025399998E-2</v>
+      </c>
+      <c r="D69" s="4">
+        <v>7.2072480085199994E-2</v>
+      </c>
     </row>
     <row r="70" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B70" s="4">
         <v>0.135315578214</v>
       </c>
-      <c r="C70" s="4"/>
-      <c r="D70" s="4"/>
+      <c r="C70" s="4">
+        <v>7.6099921372599993E-2</v>
+      </c>
+      <c r="D70" s="4">
+        <v>7.1153292029099993E-2</v>
+      </c>
     </row>
     <row r="71" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B71" s="4">
         <v>0.133696067063</v>
       </c>
-      <c r="C71" s="4"/>
-      <c r="D71" s="4"/>
+      <c r="C71" s="4">
+        <v>7.4906978972400007E-2</v>
+      </c>
+      <c r="D71" s="4">
+        <v>7.02615246316E-2</v>
+      </c>
     </row>
     <row r="72" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B72" s="4">
         <v>0.13211974806900001</v>
       </c>
-      <c r="C72" s="4"/>
-      <c r="D72" s="4"/>
+      <c r="C72" s="4">
+        <v>7.3754047759999997E-2</v>
+      </c>
+      <c r="D72" s="4">
+        <v>6.9396613885699995E-2</v>
+      </c>
     </row>
     <row r="73" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B73" s="4">
         <v>0.13058624589100001</v>
       </c>
-      <c r="C73" s="4"/>
-      <c r="D73" s="4"/>
+      <c r="C73" s="4">
+        <v>7.2639750484300006E-2</v>
+      </c>
+      <c r="D73" s="4">
+        <v>6.8558034477200006E-2</v>
+      </c>
     </row>
     <row r="74" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B74" s="4">
         <v>0.12909495548800001</v>
       </c>
-      <c r="C74" s="4"/>
-      <c r="D74" s="4"/>
+      <c r="C74" s="4">
+        <v>7.1562768551799993E-2</v>
+      </c>
+      <c r="D74" s="4">
+        <v>6.7745277134200005E-2</v>
+      </c>
     </row>
     <row r="75" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B75" s="4">
         <v>0.12764508741300001</v>
       </c>
-      <c r="C75" s="4"/>
-      <c r="D75" s="4"/>
+      <c r="C75" s="4">
+        <v>7.0521829053500004E-2</v>
+      </c>
+      <c r="D75" s="4">
+        <v>6.6957832057799996E-2</v>
+      </c>
     </row>
     <row r="76" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B76" s="4">
         <v>0.12623570887499999</v>
       </c>
-      <c r="C76" s="4"/>
-      <c r="D76" s="4"/>
+      <c r="C76" s="4">
+        <v>6.9515692761699999E-2</v>
+      </c>
+      <c r="D76" s="4">
+        <v>6.6195177861699997E-2</v>
+      </c>
     </row>
     <row r="77" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B77" s="4">
         <v>0.12486578084</v>
       </c>
-      <c r="C77" s="4"/>
-      <c r="D77" s="4"/>
+      <c r="C77" s="4">
+        <v>6.8543143900000006E-2</v>
+      </c>
+      <c r="D77" s="4">
+        <v>6.5456775102699996E-2</v>
+      </c>
     </row>
     <row r="78" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B78" s="4">
         <v>0.123534191325</v>
       </c>
-      <c r="C78" s="4"/>
-      <c r="D78" s="4"/>
+      <c r="C78" s="4">
+        <v>6.7602982383699994E-2</v>
+      </c>
+      <c r="D78" s="4">
+        <v>6.4742063368800007E-2</v>
+      </c>
     </row>
     <row r="79" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B79" s="4">
         <v>0.12223978516300001</v>
       </c>
-      <c r="C79" s="4"/>
-      <c r="D79" s="4"/>
+      <c r="C79" s="4">
+        <v>6.66940189765E-2</v>
+      </c>
+      <c r="D79" s="4">
+        <v>6.4050460942099999E-2</v>
+      </c>
     </row>
     <row r="80" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B80" s="4">
         <v>0.12098139074600001</v>
       </c>
-      <c r="C80" s="4"/>
-      <c r="D80" s="4"/>
+      <c r="C80" s="4">
+        <v>6.5815073464700002E-2</v>
+      </c>
+      <c r="D80" s="4">
+        <v>6.3381366199000005E-2</v>
+      </c>
     </row>
     <row r="81" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B81" s="4">
         <v>0.119757844332</v>
       </c>
-      <c r="C81" s="4"/>
-      <c r="D81" s="4"/>
+      <c r="C81" s="4">
+        <v>6.4964975586999998E-2</v>
+      </c>
+      <c r="D81" s="4">
+        <v>6.2734160096899999E-2</v>
+      </c>
     </row>
     <row r="82" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B82" s="4">
         <v>0.118568012184</v>
       </c>
-      <c r="C82" s="4"/>
-      <c r="D82" s="4"/>
+      <c r="C82" s="4">
+        <v>6.4142568158799998E-2</v>
+      </c>
+      <c r="D82" s="4">
+        <v>6.2108209284400001E-2</v>
+      </c>
     </row>
     <row r="83" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B83" s="4">
         <v>0.117410809561</v>
       </c>
-      <c r="C83" s="4"/>
-      <c r="D83" s="4"/>
+      <c r="C83" s="4">
+        <v>6.3346711663100005E-2</v>
+      </c>
+      <c r="D83" s="4">
+        <v>6.1502869534900001E-2</v>
+      </c>
     </row>
     <row r="84" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B84" s="4">
         <v>0.116285213582</v>
       </c>
-      <c r="C84" s="4"/>
-      <c r="D84" s="4"/>
+      <c r="C84" s="4">
+        <v>6.2576289552600001E-2</v>
+      </c>
+      <c r="D84" s="4">
+        <v>6.0917489332299998E-2</v>
+      </c>
     </row>
     <row r="85" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B85" s="4">
         <v>0.115190264619</v>
       </c>
-      <c r="C85" s="4"/>
-      <c r="D85" s="4"/>
+      <c r="C85" s="4">
+        <v>6.1830213590699998E-2</v>
+      </c>
+      <c r="D85" s="4">
+        <v>6.03514135291E-2</v>
+      </c>
     </row>
     <row r="86" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B86" s="4">
         <v>0.114125049617</v>
       </c>
-      <c r="C86" s="4"/>
-      <c r="D86" s="4"/>
+      <c r="C86" s="4">
+        <v>6.1107428716999999E-2</v>
+      </c>
+      <c r="D86" s="4">
+        <v>5.9803987046599998E-2</v>
+      </c>
     </row>
     <row r="87" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B87" s="4">
         <v>0.113088662285</v>
       </c>
-      <c r="C87" s="4"/>
+      <c r="C87" s="4">
+        <v>6.0406917099999999E-2</v>
+      </c>
       <c r="D87" s="4"/>
     </row>
     <row r="88" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B88" s="4">
         <v>0.112080140715</v>
       </c>
-      <c r="C88" s="4"/>
+      <c r="C88" s="4">
+        <v>5.9727701198199999E-2</v>
+      </c>
       <c r="D88" s="4"/>
     </row>
     <row r="89" spans="2:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Comments refactored, best parameters found and benchmark updated
</commit_message>
<xml_diff>
--- a/benchmark.xlsx
+++ b/benchmark.xlsx
@@ -9854,8 +9854,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L201"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="L7" sqref="L7:L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9892,9 +9892,15 @@
       <c r="I1" s="2">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
+      <c r="J1" s="2">
+        <v>0.04</v>
+      </c>
+      <c r="K1" s="2">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="L1" s="2">
+        <v>3.5000000000000003E-2</v>
+      </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -9924,9 +9930,15 @@
       <c r="I2" s="3">
         <v>0.01</v>
       </c>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3"/>
+      <c r="J2" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="K2" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="L2" s="3">
+        <v>0.01</v>
+      </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
@@ -9956,9 +9968,15 @@
       <c r="I3" s="3">
         <v>10</v>
       </c>
-      <c r="J3" s="3"/>
-      <c r="K3" s="3"/>
-      <c r="L3" s="3"/>
+      <c r="J3" s="3">
+        <v>10</v>
+      </c>
+      <c r="K3" s="3">
+        <v>10</v>
+      </c>
+      <c r="L3" s="3">
+        <v>10</v>
+      </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
@@ -9988,9 +10006,15 @@
       <c r="I4" s="3">
         <v>42000</v>
       </c>
-      <c r="J4" s="3"/>
-      <c r="K4" s="3"/>
-      <c r="L4" s="3"/>
+      <c r="J4" s="3">
+        <v>42000</v>
+      </c>
+      <c r="K4" s="3">
+        <v>42000</v>
+      </c>
+      <c r="L4" s="3">
+        <v>42000</v>
+      </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
@@ -10020,9 +10044,15 @@
       <c r="I5" s="3">
         <v>0.87909999999999999</v>
       </c>
-      <c r="J5" s="3"/>
-      <c r="K5" s="3"/>
-      <c r="L5" s="3"/>
+      <c r="J5" s="3">
+        <v>0.89570000000000005</v>
+      </c>
+      <c r="K5" s="3">
+        <v>0.90569999999999995</v>
+      </c>
+      <c r="L5" s="3">
+        <v>0.90539999999999998</v>
+      </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
@@ -10052,9 +10082,15 @@
       <c r="I6" s="3">
         <v>39</v>
       </c>
-      <c r="J6" s="3"/>
-      <c r="K6" s="3"/>
-      <c r="L6" s="3"/>
+      <c r="J6" s="3">
+        <v>55.887999999999998</v>
+      </c>
+      <c r="K6" s="3">
+        <v>97.96</v>
+      </c>
+      <c r="L6" s="3">
+        <v>98.32</v>
+      </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B7" s="4">
@@ -10081,7 +10117,15 @@
       <c r="I7">
         <v>0.31509557605499999</v>
       </c>
-      <c r="L7" s="3"/>
+      <c r="J7">
+        <v>0.29132332332600003</v>
+      </c>
+      <c r="K7">
+        <v>0.28970615960599999</v>
+      </c>
+      <c r="L7" s="3">
+        <v>0.27472683345100002</v>
+      </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B8" s="4">
@@ -10108,6 +10152,15 @@
       <c r="I8">
         <v>0.15276374786399999</v>
       </c>
+      <c r="J8">
+        <v>0.14866008000700001</v>
+      </c>
+      <c r="K8">
+        <v>0.13067017907299999</v>
+      </c>
+      <c r="L8">
+        <v>0.107005001265</v>
+      </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B9" s="4">
@@ -10134,6 +10187,15 @@
       <c r="I9">
         <v>9.6804142683600006E-2</v>
       </c>
+      <c r="J9">
+        <v>0.101321125991</v>
+      </c>
+      <c r="K9">
+        <v>7.5256636925300005E-2</v>
+      </c>
+      <c r="L9">
+        <v>6.2803935533399996E-2</v>
+      </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B10" s="4">
@@ -10160,6 +10222,15 @@
       <c r="I10">
         <v>7.0518594195800005E-2</v>
       </c>
+      <c r="J10">
+        <v>6.9843638730099994E-2</v>
+      </c>
+      <c r="K10">
+        <v>5.3899718771999998E-2</v>
+      </c>
+      <c r="L10">
+        <v>4.6790040014900003E-2</v>
+      </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B11" s="4">
@@ -10186,6 +10257,15 @@
       <c r="I11">
         <v>5.6831463220600002E-2</v>
       </c>
+      <c r="J11">
+        <v>5.4634392477199999E-2</v>
+      </c>
+      <c r="K11">
+        <v>4.40263225528E-2</v>
+      </c>
+      <c r="L11">
+        <v>3.9773475451199997E-2</v>
+      </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B12" s="4">
@@ -10209,6 +10289,15 @@
       <c r="H12">
         <v>0.14656990323800001</v>
       </c>
+      <c r="J12">
+        <v>4.6768262714400002E-2</v>
+      </c>
+      <c r="K12">
+        <v>3.8464975454499999E-2</v>
+      </c>
+      <c r="L12">
+        <v>3.6086898515099997E-2</v>
+      </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B13" s="4">
@@ -10232,6 +10321,15 @@
       <c r="H13">
         <v>0.13359360717999999</v>
       </c>
+      <c r="J13">
+        <v>4.2126833976999997E-2</v>
+      </c>
+      <c r="K13">
+        <v>3.4987927439100001E-2</v>
+      </c>
+      <c r="L13">
+        <v>3.3919647220099998E-2</v>
+      </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B14" s="4">
@@ -10254,6 +10352,9 @@
       </c>
       <c r="H14">
         <v>0.12081348240299999</v>
+      </c>
+      <c r="J14">
+        <v>3.9083675220499998E-2</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">

</xml_diff>